<commit_message>
Update the reference assembly in the metadata spreadsheet before brokering
</commit_message>
<xml_diff>
--- a/tests/resources/metadata_2_analysis.xlsx
+++ b/tests/resources/metadata_2_analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcezard/PycharmProjects/eva-submission/tests/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94188D8-640A-3441-AC66-0B72F0D2AC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA21E11-3AC5-AA4B-857A-5BF0F6EAACBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8460" yWindow="4100" windowWidth="23260" windowHeight="12580" tabRatio="500" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8460" yWindow="4100" windowWidth="23260" windowHeight="12580" tabRatio="500" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLEASE READ FIRST" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,12 @@
     <sheet name="Files" sheetId="10" r:id="rId10"/>
     <sheet name="CVs" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="776">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="777">
   <si>
     <t>PLEASE READ FIRST</t>
   </si>
@@ -2359,6 +2359,9 @@
   </si>
   <si>
     <t>T202.vcf.gz.tbi</t>
+  </si>
+  <si>
+    <t>GCA_000001405</t>
   </si>
 </sst>
 </file>
@@ -2743,7 +2746,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2847,7 +2850,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2866,22 +2868,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2892,12 +2878,27 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3267,7 +3268,7 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:AMK23"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection sqref="A1:B1"/>
@@ -3277,21 +3278,21 @@
   <cols>
     <col min="1" max="1" width="29" style="1" customWidth="1"/>
     <col min="2" max="2" width="255.5" style="1" customWidth="1"/>
-    <col min="3" max="1025" width="10.83203125" style="51" customWidth="1"/>
+    <col min="3" max="1025" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="65"/>
+      <c r="A1" s="69"/>
       <c r="B1" s="66"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
     </row>
     <row r="2" spans="1:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="72" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="66"/>
@@ -3303,7 +3304,7 @@
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="68" t="s">
+      <c r="A3" s="73" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="66"/>
@@ -3315,41 +3316,41 @@
       <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:8" s="4" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="69" t="s">
+      <c r="A4" s="68" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="66"/>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="65"/>
+      <c r="A5" s="69"/>
       <c r="B5" s="66"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="63"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
     </row>
     <row r="6" spans="1:8" s="4" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="62" t="s">
+      <c r="A6" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="62"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="61"/>
     </row>
     <row r="7" spans="1:8" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="72" t="s">
+      <c r="A7" s="65" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="66"/>
@@ -3361,42 +3362,42 @@
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="73"/>
+      <c r="A8" s="67"/>
       <c r="B8" s="66"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="63"/>
-      <c r="H8" s="63"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
     </row>
     <row r="9" spans="1:8" s="4" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="69" t="s">
+      <c r="A9" s="68" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="66"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="63"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="62"/>
     </row>
     <row r="10" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="65"/>
+      <c r="A10" s="69"/>
       <c r="B10" s="66"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="63"/>
-      <c r="H10" s="63"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="62"/>
     </row>
     <row r="11" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="74" t="s">
+      <c r="A11" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="75"/>
+      <c r="B11" s="71"/>
     </row>
     <row r="12" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
@@ -3448,28 +3449,28 @@
       </c>
     </row>
     <row r="19" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="70" t="s">
+      <c r="A19" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="71"/>
+      <c r="B19" s="64"/>
     </row>
     <row r="20" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="70" t="s">
+      <c r="A20" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="71"/>
+      <c r="B20" s="64"/>
     </row>
     <row r="21" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="70" t="s">
+      <c r="A21" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="71"/>
+      <c r="B21" s="64"/>
     </row>
     <row r="22" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="70" t="s">
+      <c r="A22" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="71"/>
+      <c r="B22" s="64"/>
     </row>
     <row r="23" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8"/>
@@ -3478,6 +3479,11 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="qXS9mSszo6ZK4PVLf2a4mgrLN9LTYf+uHOdaWY7gal7eLQi1TYc4PKeNVhIGj1PsRxEc/Fk3JaqC7G3YqwmFZQ==" saltValue="v8qTKlsQPInt8A+7GIueog==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
@@ -3487,11 +3493,6 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3500,19 +3501,19 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:AMK13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="51" customWidth="1"/>
-    <col min="2" max="2" width="33.33203125" style="51" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" style="51" customWidth="1"/>
-    <col min="4" max="4" width="33" style="51" customWidth="1"/>
-    <col min="5" max="1025" width="8.6640625" style="51" customWidth="1"/>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="33" customWidth="1"/>
+    <col min="5" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -3530,170 +3531,170 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="51" t="s">
+      <c r="A2" t="s">
         <v>149</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" t="s">
         <v>762</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" t="s">
         <v>462</v>
       </c>
-      <c r="D2" s="51" t="s">
+      <c r="D2" t="s">
         <v>763</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="51" t="s">
+      <c r="A3" t="s">
         <v>149</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" t="s">
         <v>764</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" t="s">
         <v>463</v>
       </c>
-      <c r="D3" s="51" t="s">
+      <c r="D3" t="s">
         <v>765</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="64" t="s">
+      <c r="A4" t="s">
         <v>149</v>
       </c>
-      <c r="B4" s="64" t="s">
+      <c r="B4" t="s">
         <v>768</v>
       </c>
-      <c r="C4" s="64" t="s">
+      <c r="C4" t="s">
         <v>462</v>
       </c>
-      <c r="D4" s="64" t="s">
+      <c r="D4" t="s">
         <v>763</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="64" t="s">
+      <c r="A5" t="s">
         <v>149</v>
       </c>
-      <c r="B5" s="64" t="s">
+      <c r="B5" t="s">
         <v>769</v>
       </c>
-      <c r="C5" s="64" t="s">
+      <c r="C5" t="s">
         <v>463</v>
       </c>
-      <c r="D5" s="64" t="s">
+      <c r="D5" t="s">
         <v>765</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="64" t="s">
+      <c r="A6" t="s">
         <v>149</v>
       </c>
-      <c r="B6" s="64" t="s">
+      <c r="B6" t="s">
         <v>770</v>
       </c>
-      <c r="C6" s="64" t="s">
+      <c r="C6" t="s">
         <v>462</v>
       </c>
-      <c r="D6" s="64" t="s">
+      <c r="D6" t="s">
         <v>763</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="64" t="s">
+      <c r="A7" t="s">
         <v>149</v>
       </c>
-      <c r="B7" s="64" t="s">
+      <c r="B7" t="s">
         <v>771</v>
       </c>
-      <c r="C7" s="64" t="s">
+      <c r="C7" t="s">
         <v>463</v>
       </c>
-      <c r="D7" s="64" t="s">
+      <c r="D7" t="s">
         <v>765</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="64" t="s">
+      <c r="A8" t="s">
         <v>761</v>
       </c>
-      <c r="B8" s="64" t="s">
+      <c r="B8" t="s">
         <v>766</v>
       </c>
-      <c r="C8" s="64" t="s">
+      <c r="C8" t="s">
         <v>462</v>
       </c>
-      <c r="D8" s="64" t="s">
+      <c r="D8" t="s">
         <v>763</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="64" t="s">
+      <c r="A9" t="s">
         <v>761</v>
       </c>
-      <c r="B9" s="64" t="s">
+      <c r="B9" t="s">
         <v>767</v>
       </c>
-      <c r="C9" s="64" t="s">
+      <c r="C9" t="s">
         <v>463</v>
       </c>
-      <c r="D9" s="64" t="s">
+      <c r="D9" t="s">
         <v>765</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="51" t="s">
+      <c r="A10" t="s">
         <v>761</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" t="s">
         <v>772</v>
       </c>
-      <c r="C10" s="51" t="s">
+      <c r="C10" t="s">
         <v>462</v>
       </c>
-      <c r="D10" s="51" t="s">
+      <c r="D10" t="s">
         <v>763</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="51" t="s">
+      <c r="A11" t="s">
         <v>761</v>
       </c>
-      <c r="B11" s="51" t="s">
+      <c r="B11" t="s">
         <v>773</v>
       </c>
-      <c r="C11" s="51" t="s">
+      <c r="C11" t="s">
         <v>463</v>
       </c>
-      <c r="D11" s="51" t="s">
+      <c r="D11" t="s">
         <v>765</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="64" t="s">
+      <c r="A12" t="s">
         <v>761</v>
       </c>
-      <c r="B12" s="64" t="s">
+      <c r="B12" t="s">
         <v>774</v>
       </c>
-      <c r="C12" s="64" t="s">
+      <c r="C12" t="s">
         <v>462</v>
       </c>
-      <c r="D12" s="64" t="s">
+      <c r="D12" t="s">
         <v>763</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="64" t="s">
+      <c r="A13" t="s">
         <v>761</v>
       </c>
-      <c r="B13" s="64" t="s">
+      <c r="B13" t="s">
         <v>775</v>
       </c>
-      <c r="C13" s="64" t="s">
+      <c r="C13" t="s">
         <v>463</v>
       </c>
-      <c r="D13" s="64" t="s">
+      <c r="D13" t="s">
         <v>765</v>
       </c>
     </row>
@@ -3712,20 +3713,20 @@
   <sheetPr>
     <tabColor rgb="FFB3A2C7"/>
   </sheetPr>
-  <dimension ref="A1:AMJ281"/>
+  <dimension ref="A1:G281"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" style="51" customWidth="1"/>
-    <col min="2" max="2" width="39" style="51" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" style="51" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" style="51" customWidth="1"/>
-    <col min="5" max="5" width="25" style="51" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" style="51" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" style="51" customWidth="1"/>
-    <col min="8" max="1024" width="8.6640625" style="51" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="2" max="2" width="39" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="8" max="1024" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -5372,7 +5373,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMK2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -5380,14 +5381,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="51" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" style="51" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" style="51" customWidth="1"/>
-    <col min="4" max="4" width="22.1640625" style="51" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="51" customWidth="1"/>
-    <col min="6" max="6" width="43.1640625" style="51" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="67.6640625" style="51" bestFit="1" customWidth="1"/>
-    <col min="8" max="1025" width="8.6640625" style="51" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" customWidth="1"/>
+    <col min="4" max="4" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="43.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="67.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -5420,10 +5421,10 @@
       <c r="B2" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="59" t="s">
+      <c r="C2" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="60" t="s">
+      <c r="D2" s="59" t="s">
         <v>33</v>
       </c>
       <c r="E2" t="s">
@@ -5450,7 +5451,7 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:AMK16"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -5458,9 +5459,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="51" customWidth="1"/>
-    <col min="2" max="2" width="176.6640625" style="51" customWidth="1"/>
-    <col min="3" max="1025" width="8.6640625" style="51" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="176.6640625" customWidth="1"/>
+    <col min="3" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -5600,7 +5601,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AMK2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -5608,21 +5609,21 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.6640625" style="51" customWidth="1"/>
-    <col min="2" max="2" width="11.5" style="51" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" style="51" customWidth="1"/>
-    <col min="4" max="4" width="6.5" style="51" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.33203125" style="51" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" style="51" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" style="51" customWidth="1"/>
-    <col min="8" max="8" width="13.5" style="51" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" style="51" customWidth="1"/>
-    <col min="10" max="10" width="40.5" style="51" customWidth="1"/>
+    <col min="1" max="1" width="36.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.5" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" customWidth="1"/>
+    <col min="10" max="10" width="40.5" customWidth="1"/>
     <col min="11" max="11" width="16.6640625" style="30" customWidth="1"/>
-    <col min="12" max="12" width="64.6640625" style="51" customWidth="1"/>
-    <col min="13" max="14" width="6" style="51" customWidth="1"/>
-    <col min="15" max="15" width="6.6640625" style="51" customWidth="1"/>
-    <col min="16" max="1025" width="8.6640625" style="51" customWidth="1"/>
+    <col min="12" max="12" width="64.6640625" customWidth="1"/>
+    <col min="13" max="14" width="6" customWidth="1"/>
+    <col min="15" max="15" width="6.6640625" customWidth="1"/>
+    <col min="16" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
@@ -5673,7 +5674,7 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="60" t="s">
         <v>68</v>
       </c>
       <c r="B2" t="s">
@@ -5703,15 +5704,15 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:AMK71"/>
+  <dimension ref="A1:B71"/>
   <sheetViews>
     <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25" style="51" customWidth="1"/>
-    <col min="2" max="2" width="164.6640625" style="51" customWidth="1"/>
-    <col min="3" max="1025" width="8.6640625" style="51" customWidth="1"/>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="164.6640625" customWidth="1"/>
+    <col min="3" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -6111,29 +6112,29 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:AMJ3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" style="51" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" style="51" customWidth="1"/>
-    <col min="3" max="3" width="40.1640625" style="51" customWidth="1"/>
-    <col min="4" max="4" width="36" style="51" customWidth="1"/>
-    <col min="5" max="5" width="23.1640625" style="51" customWidth="1"/>
-    <col min="6" max="7" width="17.1640625" style="51" customWidth="1"/>
-    <col min="8" max="8" width="29" style="51" customWidth="1"/>
-    <col min="9" max="9" width="151.6640625" style="51" customWidth="1"/>
-    <col min="10" max="10" width="10.1640625" style="51" customWidth="1"/>
-    <col min="11" max="11" width="7.5" style="51" customWidth="1"/>
-    <col min="12" max="12" width="6.6640625" style="51" customWidth="1"/>
-    <col min="13" max="13" width="8.6640625" style="51" customWidth="1"/>
-    <col min="14" max="14" width="6.5" style="51" customWidth="1"/>
-    <col min="15" max="15" width="14.6640625" style="51" customWidth="1"/>
-    <col min="16" max="1024" width="8.6640625" style="51" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" customWidth="1"/>
+    <col min="3" max="3" width="40.1640625" customWidth="1"/>
+    <col min="4" max="4" width="36" customWidth="1"/>
+    <col min="5" max="5" width="23.1640625" customWidth="1"/>
+    <col min="6" max="7" width="17.1640625" customWidth="1"/>
+    <col min="8" max="8" width="29" customWidth="1"/>
+    <col min="9" max="9" width="151.6640625" customWidth="1"/>
+    <col min="10" max="10" width="10.1640625" customWidth="1"/>
+    <col min="11" max="11" width="7.5" customWidth="1"/>
+    <col min="12" max="12" width="6.6640625" customWidth="1"/>
+    <col min="13" max="13" width="8.6640625" customWidth="1"/>
+    <col min="14" max="14" width="6.5" customWidth="1"/>
+    <col min="15" max="15" width="14.6640625" customWidth="1"/>
+    <col min="16" max="1024" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
@@ -6183,44 +6184,44 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="61" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="60" t="s">
         <v>148</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" t="s">
         <v>149</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" t="s">
         <v>150</v>
       </c>
-      <c r="D2" s="61" t="s">
+      <c r="D2" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="E2" s="51" t="s">
+      <c r="E2" t="s">
         <v>151</v>
       </c>
-      <c r="F2" s="51" t="s">
+      <c r="F2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="61" t="s">
+    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="60" t="s">
         <v>760</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" t="s">
         <v>761</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" t="s">
         <v>150</v>
       </c>
-      <c r="D3" s="61" t="s">
+      <c r="D3" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="51" t="s">
+      <c r="E3" t="s">
         <v>151</v>
       </c>
-      <c r="F3" s="51" t="s">
-        <v>152</v>
+      <c r="F3" t="s">
+        <v>776</v>
       </c>
     </row>
   </sheetData>
@@ -6237,15 +6238,15 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:AMK56"/>
+  <dimension ref="A1:B56"/>
   <sheetViews>
     <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.6640625" style="51" customWidth="1"/>
-    <col min="2" max="2" width="212" style="51" customWidth="1"/>
-    <col min="3" max="1025" width="8.6640625" style="51" customWidth="1"/>
+    <col min="1" max="1" width="44.6640625" customWidth="1"/>
+    <col min="2" max="2" width="212" customWidth="1"/>
+    <col min="3" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -6681,7 +6682,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:AMK103"/>
+  <dimension ref="A1:AT103"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A51" sqref="A51"/>
@@ -6689,165 +6690,165 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="51" customWidth="1"/>
-    <col min="2" max="3" width="16" style="51" customWidth="1"/>
-    <col min="4" max="4" width="18.5" style="51" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" style="51" customWidth="1"/>
-    <col min="6" max="6" width="14.5" style="51" customWidth="1"/>
-    <col min="7" max="7" width="23.1640625" style="51" customWidth="1"/>
-    <col min="8" max="8" width="62.5" style="51" customWidth="1"/>
-    <col min="9" max="9" width="17.5" style="51" customWidth="1"/>
-    <col min="10" max="10" width="8.1640625" style="51" customWidth="1"/>
-    <col min="11" max="11" width="12.1640625" style="51" customWidth="1"/>
-    <col min="12" max="12" width="6.1640625" style="51" customWidth="1"/>
-    <col min="13" max="13" width="14.1640625" style="51" customWidth="1"/>
-    <col min="14" max="14" width="14" style="51" customWidth="1"/>
-    <col min="15" max="15" width="13.5" style="51" customWidth="1"/>
-    <col min="16" max="16" width="11" style="51" customWidth="1"/>
-    <col min="17" max="17" width="10" style="51" customWidth="1"/>
-    <col min="18" max="18" width="9.6640625" style="51" customWidth="1"/>
-    <col min="19" max="19" width="9.5" style="51" customWidth="1"/>
-    <col min="20" max="20" width="8.5" style="51" customWidth="1"/>
-    <col min="21" max="21" width="9" style="51" customWidth="1"/>
-    <col min="22" max="22" width="10.6640625" style="51" customWidth="1"/>
-    <col min="23" max="23" width="11.5" style="51" customWidth="1"/>
-    <col min="24" max="24" width="15.6640625" style="51" customWidth="1"/>
-    <col min="25" max="26" width="16.6640625" style="51" customWidth="1"/>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="7" max="7" width="23.1640625" customWidth="1"/>
+    <col min="8" max="8" width="62.5" customWidth="1"/>
+    <col min="9" max="9" width="17.5" customWidth="1"/>
+    <col min="10" max="10" width="8.1640625" customWidth="1"/>
+    <col min="11" max="11" width="12.1640625" customWidth="1"/>
+    <col min="12" max="12" width="6.1640625" customWidth="1"/>
+    <col min="13" max="13" width="14.1640625" customWidth="1"/>
+    <col min="14" max="14" width="14" customWidth="1"/>
+    <col min="15" max="15" width="13.5" customWidth="1"/>
+    <col min="16" max="16" width="11" customWidth="1"/>
+    <col min="17" max="17" width="10" customWidth="1"/>
+    <col min="18" max="18" width="9.6640625" customWidth="1"/>
+    <col min="19" max="19" width="9.5" customWidth="1"/>
+    <col min="20" max="20" width="8.5" customWidth="1"/>
+    <col min="21" max="21" width="9" customWidth="1"/>
+    <col min="22" max="22" width="10.6640625" customWidth="1"/>
+    <col min="23" max="23" width="11.5" customWidth="1"/>
+    <col min="24" max="24" width="15.6640625" customWidth="1"/>
+    <col min="25" max="26" width="16.6640625" customWidth="1"/>
     <col min="27" max="27" width="13.83203125" style="30" customWidth="1"/>
-    <col min="28" max="28" width="34.33203125" style="51" customWidth="1"/>
-    <col min="29" max="29" width="33.6640625" style="51" customWidth="1"/>
-    <col min="30" max="30" width="4.6640625" style="51" customWidth="1"/>
-    <col min="31" max="31" width="12" style="51" customWidth="1"/>
-    <col min="32" max="32" width="14.6640625" style="51" customWidth="1"/>
-    <col min="33" max="33" width="6.6640625" style="51" customWidth="1"/>
-    <col min="34" max="34" width="8.1640625" style="51" customWidth="1"/>
-    <col min="35" max="35" width="20" style="51" customWidth="1"/>
-    <col min="36" max="36" width="7.1640625" style="51" customWidth="1"/>
-    <col min="37" max="37" width="7.6640625" style="51" customWidth="1"/>
-    <col min="38" max="38" width="6.6640625" style="51" customWidth="1"/>
-    <col min="39" max="39" width="5.6640625" style="51" customWidth="1"/>
-    <col min="40" max="40" width="11" style="51" customWidth="1"/>
-    <col min="41" max="41" width="6.6640625" style="51" customWidth="1"/>
-    <col min="42" max="42" width="9.6640625" style="51" customWidth="1"/>
-    <col min="43" max="43" width="8" style="51" customWidth="1"/>
-    <col min="44" max="44" width="8.1640625" style="51" customWidth="1"/>
-    <col min="45" max="45" width="19.1640625" style="51" customWidth="1"/>
-    <col min="46" max="46" width="15.6640625" style="51" customWidth="1"/>
-    <col min="47" max="1025" width="8.6640625" style="51" customWidth="1"/>
+    <col min="28" max="28" width="34.33203125" customWidth="1"/>
+    <col min="29" max="29" width="33.6640625" customWidth="1"/>
+    <col min="30" max="30" width="4.6640625" customWidth="1"/>
+    <col min="31" max="31" width="12" customWidth="1"/>
+    <col min="32" max="32" width="14.6640625" customWidth="1"/>
+    <col min="33" max="33" width="6.6640625" customWidth="1"/>
+    <col min="34" max="34" width="8.1640625" customWidth="1"/>
+    <col min="35" max="35" width="20" customWidth="1"/>
+    <col min="36" max="36" width="7.1640625" customWidth="1"/>
+    <col min="37" max="37" width="7.6640625" customWidth="1"/>
+    <col min="38" max="38" width="6.6640625" customWidth="1"/>
+    <col min="39" max="39" width="5.6640625" customWidth="1"/>
+    <col min="40" max="40" width="11" customWidth="1"/>
+    <col min="41" max="41" width="6.6640625" customWidth="1"/>
+    <col min="42" max="42" width="9.6640625" customWidth="1"/>
+    <col min="43" max="43" width="8" customWidth="1"/>
+    <col min="44" max="44" width="8.1640625" customWidth="1"/>
+    <col min="45" max="45" width="19.1640625" customWidth="1"/>
+    <col min="46" max="46" width="15.6640625" customWidth="1"/>
+    <col min="47" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A1" s="49"/>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="77" t="s">
         <v>250</v>
       </c>
-      <c r="C1" s="77"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="83"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="81"/>
       <c r="F1" s="36" t="s">
         <v>251</v>
       </c>
-      <c r="G1" s="52"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54"/>
-      <c r="AA1" s="56"/>
-      <c r="AB1" s="54"/>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="54"/>
-      <c r="AF1" s="54"/>
-      <c r="AG1" s="54"/>
-      <c r="AH1" s="54"/>
-      <c r="AI1" s="54"/>
-      <c r="AJ1" s="54"/>
-      <c r="AK1" s="54"/>
-      <c r="AL1" s="54"/>
-      <c r="AM1" s="54"/>
-      <c r="AN1" s="54"/>
-      <c r="AO1" s="54"/>
-      <c r="AP1" s="54"/>
-      <c r="AQ1" s="54"/>
-      <c r="AR1" s="54"/>
-      <c r="AS1" s="54"/>
-      <c r="AT1" s="55"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="52"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="53"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+      <c r="T1" s="53"/>
+      <c r="U1" s="53"/>
+      <c r="V1" s="53"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="53"/>
+      <c r="Y1" s="53"/>
+      <c r="Z1" s="53"/>
+      <c r="AA1" s="55"/>
+      <c r="AB1" s="53"/>
+      <c r="AC1" s="53"/>
+      <c r="AD1" s="53"/>
+      <c r="AE1" s="53"/>
+      <c r="AF1" s="53"/>
+      <c r="AG1" s="53"/>
+      <c r="AH1" s="53"/>
+      <c r="AI1" s="53"/>
+      <c r="AJ1" s="53"/>
+      <c r="AK1" s="53"/>
+      <c r="AL1" s="53"/>
+      <c r="AM1" s="53"/>
+      <c r="AN1" s="53"/>
+      <c r="AO1" s="53"/>
+      <c r="AP1" s="53"/>
+      <c r="AQ1" s="53"/>
+      <c r="AR1" s="53"/>
+      <c r="AS1" s="53"/>
+      <c r="AT1" s="54"/>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A2" s="50"/>
-      <c r="B2" s="80"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="76" t="s">
+      <c r="B2" s="78"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="74" t="s">
         <v>161</v>
       </c>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="84" t="s">
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="82" t="s">
         <v>173</v>
       </c>
-      <c r="M2" s="77"/>
-      <c r="N2" s="78"/>
-      <c r="O2" s="84" t="s">
+      <c r="M2" s="75"/>
+      <c r="N2" s="76"/>
+      <c r="O2" s="82" t="s">
         <v>180</v>
       </c>
-      <c r="P2" s="77"/>
-      <c r="Q2" s="78"/>
-      <c r="R2" s="76" t="s">
+      <c r="P2" s="75"/>
+      <c r="Q2" s="76"/>
+      <c r="R2" s="74" t="s">
         <v>185</v>
       </c>
-      <c r="S2" s="77"/>
-      <c r="T2" s="77"/>
-      <c r="U2" s="77"/>
-      <c r="V2" s="78"/>
-      <c r="W2" s="76" t="s">
+      <c r="S2" s="75"/>
+      <c r="T2" s="75"/>
+      <c r="U2" s="75"/>
+      <c r="V2" s="76"/>
+      <c r="W2" s="74" t="s">
         <v>196</v>
       </c>
-      <c r="X2" s="77"/>
-      <c r="Y2" s="78"/>
-      <c r="Z2" s="76" t="s">
+      <c r="X2" s="75"/>
+      <c r="Y2" s="76"/>
+      <c r="Z2" s="74" t="s">
         <v>203</v>
       </c>
-      <c r="AA2" s="77"/>
-      <c r="AB2" s="77"/>
-      <c r="AC2" s="77"/>
-      <c r="AD2" s="77"/>
-      <c r="AE2" s="77"/>
-      <c r="AF2" s="77"/>
-      <c r="AG2" s="77"/>
-      <c r="AH2" s="77"/>
-      <c r="AI2" s="78"/>
-      <c r="AJ2" s="76" t="s">
+      <c r="AA2" s="75"/>
+      <c r="AB2" s="75"/>
+      <c r="AC2" s="75"/>
+      <c r="AD2" s="75"/>
+      <c r="AE2" s="75"/>
+      <c r="AF2" s="75"/>
+      <c r="AG2" s="75"/>
+      <c r="AH2" s="75"/>
+      <c r="AI2" s="76"/>
+      <c r="AJ2" s="74" t="s">
         <v>224</v>
       </c>
-      <c r="AK2" s="77"/>
-      <c r="AL2" s="77"/>
-      <c r="AM2" s="77"/>
-      <c r="AN2" s="77"/>
-      <c r="AO2" s="77"/>
-      <c r="AP2" s="77"/>
-      <c r="AQ2" s="77"/>
-      <c r="AR2" s="77"/>
-      <c r="AS2" s="78"/>
+      <c r="AK2" s="75"/>
+      <c r="AL2" s="75"/>
+      <c r="AM2" s="75"/>
+      <c r="AN2" s="75"/>
+      <c r="AO2" s="75"/>
+      <c r="AP2" s="75"/>
+      <c r="AQ2" s="75"/>
+      <c r="AR2" s="75"/>
+      <c r="AS2" s="76"/>
     </row>
     <row r="3" spans="1:46" ht="26" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="37" t="s">
@@ -6928,7 +6929,7 @@
       <c r="Z3" s="47" t="s">
         <v>204</v>
       </c>
-      <c r="AA3" s="57" t="s">
+      <c r="AA3" s="56" t="s">
         <v>206</v>
       </c>
       <c r="AB3" s="44" t="s">
@@ -7056,7 +7057,7 @@
       <c r="M7" t="s">
         <v>256</v>
       </c>
-      <c r="Z7" s="58"/>
+      <c r="Z7" s="57"/>
     </row>
     <row r="8" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -7841,7 +7842,7 @@
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A54" s="51" t="s">
+      <c r="A54" t="s">
         <v>761</v>
       </c>
       <c r="F54" t="s">
@@ -7858,7 +7859,7 @@
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A55" s="51" t="s">
+      <c r="A55" t="s">
         <v>761</v>
       </c>
       <c r="F55" t="s">
@@ -7875,7 +7876,7 @@
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A56" s="51" t="s">
+      <c r="A56" t="s">
         <v>761</v>
       </c>
       <c r="F56" t="s">
@@ -7892,7 +7893,7 @@
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A57" s="51" t="s">
+      <c r="A57" t="s">
         <v>761</v>
       </c>
       <c r="F57" t="s">
@@ -7909,7 +7910,7 @@
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A58" s="51" t="s">
+      <c r="A58" t="s">
         <v>761</v>
       </c>
       <c r="F58" t="s">
@@ -7926,7 +7927,7 @@
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A59" s="51" t="s">
+      <c r="A59" t="s">
         <v>761</v>
       </c>
       <c r="F59" t="s">
@@ -7943,7 +7944,7 @@
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A60" s="51" t="s">
+      <c r="A60" t="s">
         <v>761</v>
       </c>
       <c r="F60" t="s">
@@ -7960,7 +7961,7 @@
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A61" s="51" t="s">
+      <c r="A61" t="s">
         <v>761</v>
       </c>
       <c r="F61" t="s">
@@ -7977,7 +7978,7 @@
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A62" s="51" t="s">
+      <c r="A62" t="s">
         <v>761</v>
       </c>
       <c r="F62" t="s">
@@ -7994,7 +7995,7 @@
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A63" s="51" t="s">
+      <c r="A63" t="s">
         <v>761</v>
       </c>
       <c r="F63" t="s">
@@ -8011,7 +8012,7 @@
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A64" s="51" t="s">
+      <c r="A64" t="s">
         <v>761</v>
       </c>
       <c r="F64" t="s">
@@ -8028,7 +8029,7 @@
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A65" s="51" t="s">
+      <c r="A65" t="s">
         <v>761</v>
       </c>
       <c r="F65" t="s">
@@ -8045,7 +8046,7 @@
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A66" s="51" t="s">
+      <c r="A66" t="s">
         <v>761</v>
       </c>
       <c r="F66" t="s">
@@ -8062,7 +8063,7 @@
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A67" s="51" t="s">
+      <c r="A67" t="s">
         <v>761</v>
       </c>
       <c r="F67" t="s">
@@ -8079,7 +8080,7 @@
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A68" s="51" t="s">
+      <c r="A68" t="s">
         <v>761</v>
       </c>
       <c r="F68" t="s">
@@ -8096,7 +8097,7 @@
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A69" s="51" t="s">
+      <c r="A69" t="s">
         <v>761</v>
       </c>
       <c r="F69" t="s">
@@ -8113,7 +8114,7 @@
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A70" s="51" t="s">
+      <c r="A70" t="s">
         <v>761</v>
       </c>
       <c r="F70" t="s">
@@ -8130,7 +8131,7 @@
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A71" s="51" t="s">
+      <c r="A71" t="s">
         <v>761</v>
       </c>
       <c r="F71" t="s">
@@ -8147,7 +8148,7 @@
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A72" s="51" t="s">
+      <c r="A72" t="s">
         <v>761</v>
       </c>
       <c r="F72" t="s">
@@ -8164,7 +8165,7 @@
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A73" s="51" t="s">
+      <c r="A73" t="s">
         <v>761</v>
       </c>
       <c r="F73" t="s">
@@ -8181,7 +8182,7 @@
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A74" s="51" t="s">
+      <c r="A74" t="s">
         <v>761</v>
       </c>
       <c r="F74" t="s">
@@ -8198,7 +8199,7 @@
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A75" s="51" t="s">
+      <c r="A75" t="s">
         <v>761</v>
       </c>
       <c r="F75" t="s">
@@ -8215,7 +8216,7 @@
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A76" s="51" t="s">
+      <c r="A76" t="s">
         <v>761</v>
       </c>
       <c r="F76" t="s">
@@ -8232,7 +8233,7 @@
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A77" s="51" t="s">
+      <c r="A77" t="s">
         <v>761</v>
       </c>
       <c r="F77" t="s">
@@ -8249,7 +8250,7 @@
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A78" s="51" t="s">
+      <c r="A78" t="s">
         <v>761</v>
       </c>
       <c r="F78" t="s">
@@ -8266,7 +8267,7 @@
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A79" s="51" t="s">
+      <c r="A79" t="s">
         <v>761</v>
       </c>
       <c r="F79" t="s">
@@ -8283,7 +8284,7 @@
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A80" s="51" t="s">
+      <c r="A80" t="s">
         <v>761</v>
       </c>
       <c r="F80" t="s">
@@ -8300,7 +8301,7 @@
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A81" s="51" t="s">
+      <c r="A81" t="s">
         <v>761</v>
       </c>
       <c r="F81" t="s">
@@ -8317,7 +8318,7 @@
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A82" s="51" t="s">
+      <c r="A82" t="s">
         <v>761</v>
       </c>
       <c r="F82" t="s">
@@ -8334,7 +8335,7 @@
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A83" s="51" t="s">
+      <c r="A83" t="s">
         <v>761</v>
       </c>
       <c r="F83" t="s">
@@ -8351,7 +8352,7 @@
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A84" s="51" t="s">
+      <c r="A84" t="s">
         <v>761</v>
       </c>
       <c r="F84" t="s">
@@ -8368,7 +8369,7 @@
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A85" s="51" t="s">
+      <c r="A85" t="s">
         <v>761</v>
       </c>
       <c r="F85" t="s">
@@ -8385,7 +8386,7 @@
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A86" s="51" t="s">
+      <c r="A86" t="s">
         <v>761</v>
       </c>
       <c r="F86" t="s">
@@ -8402,7 +8403,7 @@
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A87" s="51" t="s">
+      <c r="A87" t="s">
         <v>761</v>
       </c>
       <c r="F87" t="s">
@@ -8419,7 +8420,7 @@
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A88" s="51" t="s">
+      <c r="A88" t="s">
         <v>761</v>
       </c>
       <c r="F88" t="s">
@@ -8436,7 +8437,7 @@
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A89" s="51" t="s">
+      <c r="A89" t="s">
         <v>761</v>
       </c>
       <c r="F89" t="s">
@@ -8453,7 +8454,7 @@
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A90" s="51" t="s">
+      <c r="A90" t="s">
         <v>761</v>
       </c>
       <c r="F90" t="s">
@@ -8470,7 +8471,7 @@
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A91" s="51" t="s">
+      <c r="A91" t="s">
         <v>761</v>
       </c>
       <c r="F91" t="s">
@@ -8487,7 +8488,7 @@
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A92" s="51" t="s">
+      <c r="A92" t="s">
         <v>761</v>
       </c>
       <c r="F92" t="s">
@@ -8504,7 +8505,7 @@
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A93" s="51" t="s">
+      <c r="A93" t="s">
         <v>761</v>
       </c>
       <c r="F93" t="s">
@@ -8521,7 +8522,7 @@
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A94" s="51" t="s">
+      <c r="A94" t="s">
         <v>761</v>
       </c>
       <c r="F94" t="s">
@@ -8538,7 +8539,7 @@
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A95" s="51" t="s">
+      <c r="A95" t="s">
         <v>761</v>
       </c>
       <c r="F95" t="s">
@@ -8555,7 +8556,7 @@
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A96" s="51" t="s">
+      <c r="A96" t="s">
         <v>761</v>
       </c>
       <c r="F96" t="s">
@@ -8572,7 +8573,7 @@
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A97" s="51" t="s">
+      <c r="A97" t="s">
         <v>761</v>
       </c>
       <c r="F97" t="s">
@@ -8589,7 +8590,7 @@
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A98" s="51" t="s">
+      <c r="A98" t="s">
         <v>761</v>
       </c>
       <c r="F98" t="s">
@@ -8606,7 +8607,7 @@
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A99" s="51" t="s">
+      <c r="A99" t="s">
         <v>761</v>
       </c>
       <c r="F99" t="s">
@@ -8623,7 +8624,7 @@
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A100" s="51" t="s">
+      <c r="A100" t="s">
         <v>761</v>
       </c>
       <c r="F100" t="s">
@@ -8640,7 +8641,7 @@
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A101" s="51" t="s">
+      <c r="A101" t="s">
         <v>761</v>
       </c>
       <c r="F101" t="s">
@@ -8657,7 +8658,7 @@
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A102" s="51" t="s">
+      <c r="A102" t="s">
         <v>761</v>
       </c>
       <c r="F102" t="s">
@@ -8674,7 +8675,7 @@
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A103" s="51" t="s">
+      <c r="A103" t="s">
         <v>761</v>
       </c>
       <c r="F103" t="s">
@@ -8717,15 +8718,15 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:AMK5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" style="51" customWidth="1"/>
-    <col min="2" max="2" width="114.6640625" style="51" customWidth="1"/>
-    <col min="3" max="1025" width="8.6640625" style="51" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="114.6640625" customWidth="1"/>
+    <col min="3" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fix from submission (#168)
* Ensure unique analysis when writing to spreadsheet
* Fix link retrieval from upload single file to ENA
* Fix validation of date in metadata
* Update the reference assembly in the metadata spreadsheet before brokering
</commit_message>
<xml_diff>
--- a/tests/resources/metadata_2_analysis.xlsx
+++ b/tests/resources/metadata_2_analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcezard/PycharmProjects/eva-submission/tests/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94188D8-640A-3441-AC66-0B72F0D2AC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA21E11-3AC5-AA4B-857A-5BF0F6EAACBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8460" yWindow="4100" windowWidth="23260" windowHeight="12580" tabRatio="500" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8460" yWindow="4100" windowWidth="23260" windowHeight="12580" tabRatio="500" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLEASE READ FIRST" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,12 @@
     <sheet name="Files" sheetId="10" r:id="rId10"/>
     <sheet name="CVs" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="776">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="777">
   <si>
     <t>PLEASE READ FIRST</t>
   </si>
@@ -2359,6 +2359,9 @@
   </si>
   <si>
     <t>T202.vcf.gz.tbi</t>
+  </si>
+  <si>
+    <t>GCA_000001405</t>
   </si>
 </sst>
 </file>
@@ -2743,7 +2746,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2847,7 +2850,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2866,22 +2868,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2892,12 +2878,27 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3267,7 +3268,7 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:AMK23"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection sqref="A1:B1"/>
@@ -3277,21 +3278,21 @@
   <cols>
     <col min="1" max="1" width="29" style="1" customWidth="1"/>
     <col min="2" max="2" width="255.5" style="1" customWidth="1"/>
-    <col min="3" max="1025" width="10.83203125" style="51" customWidth="1"/>
+    <col min="3" max="1025" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="65"/>
+      <c r="A1" s="69"/>
       <c r="B1" s="66"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
     </row>
     <row r="2" spans="1:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="72" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="66"/>
@@ -3303,7 +3304,7 @@
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="68" t="s">
+      <c r="A3" s="73" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="66"/>
@@ -3315,41 +3316,41 @@
       <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:8" s="4" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="69" t="s">
+      <c r="A4" s="68" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="66"/>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="65"/>
+      <c r="A5" s="69"/>
       <c r="B5" s="66"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="63"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
     </row>
     <row r="6" spans="1:8" s="4" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="62" t="s">
+      <c r="A6" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="62"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="61"/>
     </row>
     <row r="7" spans="1:8" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="72" t="s">
+      <c r="A7" s="65" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="66"/>
@@ -3361,42 +3362,42 @@
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="73"/>
+      <c r="A8" s="67"/>
       <c r="B8" s="66"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="63"/>
-      <c r="H8" s="63"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
     </row>
     <row r="9" spans="1:8" s="4" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="69" t="s">
+      <c r="A9" s="68" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="66"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="63"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="62"/>
     </row>
     <row r="10" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="65"/>
+      <c r="A10" s="69"/>
       <c r="B10" s="66"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="63"/>
-      <c r="H10" s="63"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="62"/>
     </row>
     <row r="11" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="74" t="s">
+      <c r="A11" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="75"/>
+      <c r="B11" s="71"/>
     </row>
     <row r="12" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
@@ -3448,28 +3449,28 @@
       </c>
     </row>
     <row r="19" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="70" t="s">
+      <c r="A19" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="71"/>
+      <c r="B19" s="64"/>
     </row>
     <row r="20" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="70" t="s">
+      <c r="A20" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="71"/>
+      <c r="B20" s="64"/>
     </row>
     <row r="21" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="70" t="s">
+      <c r="A21" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="71"/>
+      <c r="B21" s="64"/>
     </row>
     <row r="22" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="70" t="s">
+      <c r="A22" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="71"/>
+      <c r="B22" s="64"/>
     </row>
     <row r="23" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8"/>
@@ -3478,6 +3479,11 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="qXS9mSszo6ZK4PVLf2a4mgrLN9LTYf+uHOdaWY7gal7eLQi1TYc4PKeNVhIGj1PsRxEc/Fk3JaqC7G3YqwmFZQ==" saltValue="v8qTKlsQPInt8A+7GIueog==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
@@ -3487,11 +3493,6 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3500,19 +3501,19 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:AMK13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="51" customWidth="1"/>
-    <col min="2" max="2" width="33.33203125" style="51" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" style="51" customWidth="1"/>
-    <col min="4" max="4" width="33" style="51" customWidth="1"/>
-    <col min="5" max="1025" width="8.6640625" style="51" customWidth="1"/>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="33" customWidth="1"/>
+    <col min="5" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -3530,170 +3531,170 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="51" t="s">
+      <c r="A2" t="s">
         <v>149</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" t="s">
         <v>762</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" t="s">
         <v>462</v>
       </c>
-      <c r="D2" s="51" t="s">
+      <c r="D2" t="s">
         <v>763</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="51" t="s">
+      <c r="A3" t="s">
         <v>149</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" t="s">
         <v>764</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" t="s">
         <v>463</v>
       </c>
-      <c r="D3" s="51" t="s">
+      <c r="D3" t="s">
         <v>765</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="64" t="s">
+      <c r="A4" t="s">
         <v>149</v>
       </c>
-      <c r="B4" s="64" t="s">
+      <c r="B4" t="s">
         <v>768</v>
       </c>
-      <c r="C4" s="64" t="s">
+      <c r="C4" t="s">
         <v>462</v>
       </c>
-      <c r="D4" s="64" t="s">
+      <c r="D4" t="s">
         <v>763</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="64" t="s">
+      <c r="A5" t="s">
         <v>149</v>
       </c>
-      <c r="B5" s="64" t="s">
+      <c r="B5" t="s">
         <v>769</v>
       </c>
-      <c r="C5" s="64" t="s">
+      <c r="C5" t="s">
         <v>463</v>
       </c>
-      <c r="D5" s="64" t="s">
+      <c r="D5" t="s">
         <v>765</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="64" t="s">
+      <c r="A6" t="s">
         <v>149</v>
       </c>
-      <c r="B6" s="64" t="s">
+      <c r="B6" t="s">
         <v>770</v>
       </c>
-      <c r="C6" s="64" t="s">
+      <c r="C6" t="s">
         <v>462</v>
       </c>
-      <c r="D6" s="64" t="s">
+      <c r="D6" t="s">
         <v>763</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="64" t="s">
+      <c r="A7" t="s">
         <v>149</v>
       </c>
-      <c r="B7" s="64" t="s">
+      <c r="B7" t="s">
         <v>771</v>
       </c>
-      <c r="C7" s="64" t="s">
+      <c r="C7" t="s">
         <v>463</v>
       </c>
-      <c r="D7" s="64" t="s">
+      <c r="D7" t="s">
         <v>765</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="64" t="s">
+      <c r="A8" t="s">
         <v>761</v>
       </c>
-      <c r="B8" s="64" t="s">
+      <c r="B8" t="s">
         <v>766</v>
       </c>
-      <c r="C8" s="64" t="s">
+      <c r="C8" t="s">
         <v>462</v>
       </c>
-      <c r="D8" s="64" t="s">
+      <c r="D8" t="s">
         <v>763</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="64" t="s">
+      <c r="A9" t="s">
         <v>761</v>
       </c>
-      <c r="B9" s="64" t="s">
+      <c r="B9" t="s">
         <v>767</v>
       </c>
-      <c r="C9" s="64" t="s">
+      <c r="C9" t="s">
         <v>463</v>
       </c>
-      <c r="D9" s="64" t="s">
+      <c r="D9" t="s">
         <v>765</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="51" t="s">
+      <c r="A10" t="s">
         <v>761</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" t="s">
         <v>772</v>
       </c>
-      <c r="C10" s="51" t="s">
+      <c r="C10" t="s">
         <v>462</v>
       </c>
-      <c r="D10" s="51" t="s">
+      <c r="D10" t="s">
         <v>763</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="51" t="s">
+      <c r="A11" t="s">
         <v>761</v>
       </c>
-      <c r="B11" s="51" t="s">
+      <c r="B11" t="s">
         <v>773</v>
       </c>
-      <c r="C11" s="51" t="s">
+      <c r="C11" t="s">
         <v>463</v>
       </c>
-      <c r="D11" s="51" t="s">
+      <c r="D11" t="s">
         <v>765</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="64" t="s">
+      <c r="A12" t="s">
         <v>761</v>
       </c>
-      <c r="B12" s="64" t="s">
+      <c r="B12" t="s">
         <v>774</v>
       </c>
-      <c r="C12" s="64" t="s">
+      <c r="C12" t="s">
         <v>462</v>
       </c>
-      <c r="D12" s="64" t="s">
+      <c r="D12" t="s">
         <v>763</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="64" t="s">
+      <c r="A13" t="s">
         <v>761</v>
       </c>
-      <c r="B13" s="64" t="s">
+      <c r="B13" t="s">
         <v>775</v>
       </c>
-      <c r="C13" s="64" t="s">
+      <c r="C13" t="s">
         <v>463</v>
       </c>
-      <c r="D13" s="64" t="s">
+      <c r="D13" t="s">
         <v>765</v>
       </c>
     </row>
@@ -3712,20 +3713,20 @@
   <sheetPr>
     <tabColor rgb="FFB3A2C7"/>
   </sheetPr>
-  <dimension ref="A1:AMJ281"/>
+  <dimension ref="A1:G281"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" style="51" customWidth="1"/>
-    <col min="2" max="2" width="39" style="51" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" style="51" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" style="51" customWidth="1"/>
-    <col min="5" max="5" width="25" style="51" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" style="51" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" style="51" customWidth="1"/>
-    <col min="8" max="1024" width="8.6640625" style="51" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="2" max="2" width="39" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="8" max="1024" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -5372,7 +5373,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMK2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -5380,14 +5381,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="51" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" style="51" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" style="51" customWidth="1"/>
-    <col min="4" max="4" width="22.1640625" style="51" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="51" customWidth="1"/>
-    <col min="6" max="6" width="43.1640625" style="51" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="67.6640625" style="51" bestFit="1" customWidth="1"/>
-    <col min="8" max="1025" width="8.6640625" style="51" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" customWidth="1"/>
+    <col min="4" max="4" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="43.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="67.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -5420,10 +5421,10 @@
       <c r="B2" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="59" t="s">
+      <c r="C2" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="60" t="s">
+      <c r="D2" s="59" t="s">
         <v>33</v>
       </c>
       <c r="E2" t="s">
@@ -5450,7 +5451,7 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:AMK16"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -5458,9 +5459,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="51" customWidth="1"/>
-    <col min="2" max="2" width="176.6640625" style="51" customWidth="1"/>
-    <col min="3" max="1025" width="8.6640625" style="51" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="176.6640625" customWidth="1"/>
+    <col min="3" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -5600,7 +5601,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AMK2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -5608,21 +5609,21 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.6640625" style="51" customWidth="1"/>
-    <col min="2" max="2" width="11.5" style="51" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" style="51" customWidth="1"/>
-    <col min="4" max="4" width="6.5" style="51" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.33203125" style="51" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" style="51" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" style="51" customWidth="1"/>
-    <col min="8" max="8" width="13.5" style="51" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" style="51" customWidth="1"/>
-    <col min="10" max="10" width="40.5" style="51" customWidth="1"/>
+    <col min="1" max="1" width="36.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.5" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" customWidth="1"/>
+    <col min="10" max="10" width="40.5" customWidth="1"/>
     <col min="11" max="11" width="16.6640625" style="30" customWidth="1"/>
-    <col min="12" max="12" width="64.6640625" style="51" customWidth="1"/>
-    <col min="13" max="14" width="6" style="51" customWidth="1"/>
-    <col min="15" max="15" width="6.6640625" style="51" customWidth="1"/>
-    <col min="16" max="1025" width="8.6640625" style="51" customWidth="1"/>
+    <col min="12" max="12" width="64.6640625" customWidth="1"/>
+    <col min="13" max="14" width="6" customWidth="1"/>
+    <col min="15" max="15" width="6.6640625" customWidth="1"/>
+    <col min="16" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
@@ -5673,7 +5674,7 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="60" t="s">
         <v>68</v>
       </c>
       <c r="B2" t="s">
@@ -5703,15 +5704,15 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:AMK71"/>
+  <dimension ref="A1:B71"/>
   <sheetViews>
     <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25" style="51" customWidth="1"/>
-    <col min="2" max="2" width="164.6640625" style="51" customWidth="1"/>
-    <col min="3" max="1025" width="8.6640625" style="51" customWidth="1"/>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="164.6640625" customWidth="1"/>
+    <col min="3" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -6111,29 +6112,29 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:AMJ3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" style="51" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" style="51" customWidth="1"/>
-    <col min="3" max="3" width="40.1640625" style="51" customWidth="1"/>
-    <col min="4" max="4" width="36" style="51" customWidth="1"/>
-    <col min="5" max="5" width="23.1640625" style="51" customWidth="1"/>
-    <col min="6" max="7" width="17.1640625" style="51" customWidth="1"/>
-    <col min="8" max="8" width="29" style="51" customWidth="1"/>
-    <col min="9" max="9" width="151.6640625" style="51" customWidth="1"/>
-    <col min="10" max="10" width="10.1640625" style="51" customWidth="1"/>
-    <col min="11" max="11" width="7.5" style="51" customWidth="1"/>
-    <col min="12" max="12" width="6.6640625" style="51" customWidth="1"/>
-    <col min="13" max="13" width="8.6640625" style="51" customWidth="1"/>
-    <col min="14" max="14" width="6.5" style="51" customWidth="1"/>
-    <col min="15" max="15" width="14.6640625" style="51" customWidth="1"/>
-    <col min="16" max="1024" width="8.6640625" style="51" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" customWidth="1"/>
+    <col min="3" max="3" width="40.1640625" customWidth="1"/>
+    <col min="4" max="4" width="36" customWidth="1"/>
+    <col min="5" max="5" width="23.1640625" customWidth="1"/>
+    <col min="6" max="7" width="17.1640625" customWidth="1"/>
+    <col min="8" max="8" width="29" customWidth="1"/>
+    <col min="9" max="9" width="151.6640625" customWidth="1"/>
+    <col min="10" max="10" width="10.1640625" customWidth="1"/>
+    <col min="11" max="11" width="7.5" customWidth="1"/>
+    <col min="12" max="12" width="6.6640625" customWidth="1"/>
+    <col min="13" max="13" width="8.6640625" customWidth="1"/>
+    <col min="14" max="14" width="6.5" customWidth="1"/>
+    <col min="15" max="15" width="14.6640625" customWidth="1"/>
+    <col min="16" max="1024" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
@@ -6183,44 +6184,44 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="61" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="60" t="s">
         <v>148</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" t="s">
         <v>149</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" t="s">
         <v>150</v>
       </c>
-      <c r="D2" s="61" t="s">
+      <c r="D2" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="E2" s="51" t="s">
+      <c r="E2" t="s">
         <v>151</v>
       </c>
-      <c r="F2" s="51" t="s">
+      <c r="F2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="61" t="s">
+    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="60" t="s">
         <v>760</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" t="s">
         <v>761</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" t="s">
         <v>150</v>
       </c>
-      <c r="D3" s="61" t="s">
+      <c r="D3" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="51" t="s">
+      <c r="E3" t="s">
         <v>151</v>
       </c>
-      <c r="F3" s="51" t="s">
-        <v>152</v>
+      <c r="F3" t="s">
+        <v>776</v>
       </c>
     </row>
   </sheetData>
@@ -6237,15 +6238,15 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:AMK56"/>
+  <dimension ref="A1:B56"/>
   <sheetViews>
     <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.6640625" style="51" customWidth="1"/>
-    <col min="2" max="2" width="212" style="51" customWidth="1"/>
-    <col min="3" max="1025" width="8.6640625" style="51" customWidth="1"/>
+    <col min="1" max="1" width="44.6640625" customWidth="1"/>
+    <col min="2" max="2" width="212" customWidth="1"/>
+    <col min="3" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -6681,7 +6682,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:AMK103"/>
+  <dimension ref="A1:AT103"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A51" sqref="A51"/>
@@ -6689,165 +6690,165 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="51" customWidth="1"/>
-    <col min="2" max="3" width="16" style="51" customWidth="1"/>
-    <col min="4" max="4" width="18.5" style="51" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" style="51" customWidth="1"/>
-    <col min="6" max="6" width="14.5" style="51" customWidth="1"/>
-    <col min="7" max="7" width="23.1640625" style="51" customWidth="1"/>
-    <col min="8" max="8" width="62.5" style="51" customWidth="1"/>
-    <col min="9" max="9" width="17.5" style="51" customWidth="1"/>
-    <col min="10" max="10" width="8.1640625" style="51" customWidth="1"/>
-    <col min="11" max="11" width="12.1640625" style="51" customWidth="1"/>
-    <col min="12" max="12" width="6.1640625" style="51" customWidth="1"/>
-    <col min="13" max="13" width="14.1640625" style="51" customWidth="1"/>
-    <col min="14" max="14" width="14" style="51" customWidth="1"/>
-    <col min="15" max="15" width="13.5" style="51" customWidth="1"/>
-    <col min="16" max="16" width="11" style="51" customWidth="1"/>
-    <col min="17" max="17" width="10" style="51" customWidth="1"/>
-    <col min="18" max="18" width="9.6640625" style="51" customWidth="1"/>
-    <col min="19" max="19" width="9.5" style="51" customWidth="1"/>
-    <col min="20" max="20" width="8.5" style="51" customWidth="1"/>
-    <col min="21" max="21" width="9" style="51" customWidth="1"/>
-    <col min="22" max="22" width="10.6640625" style="51" customWidth="1"/>
-    <col min="23" max="23" width="11.5" style="51" customWidth="1"/>
-    <col min="24" max="24" width="15.6640625" style="51" customWidth="1"/>
-    <col min="25" max="26" width="16.6640625" style="51" customWidth="1"/>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="7" max="7" width="23.1640625" customWidth="1"/>
+    <col min="8" max="8" width="62.5" customWidth="1"/>
+    <col min="9" max="9" width="17.5" customWidth="1"/>
+    <col min="10" max="10" width="8.1640625" customWidth="1"/>
+    <col min="11" max="11" width="12.1640625" customWidth="1"/>
+    <col min="12" max="12" width="6.1640625" customWidth="1"/>
+    <col min="13" max="13" width="14.1640625" customWidth="1"/>
+    <col min="14" max="14" width="14" customWidth="1"/>
+    <col min="15" max="15" width="13.5" customWidth="1"/>
+    <col min="16" max="16" width="11" customWidth="1"/>
+    <col min="17" max="17" width="10" customWidth="1"/>
+    <col min="18" max="18" width="9.6640625" customWidth="1"/>
+    <col min="19" max="19" width="9.5" customWidth="1"/>
+    <col min="20" max="20" width="8.5" customWidth="1"/>
+    <col min="21" max="21" width="9" customWidth="1"/>
+    <col min="22" max="22" width="10.6640625" customWidth="1"/>
+    <col min="23" max="23" width="11.5" customWidth="1"/>
+    <col min="24" max="24" width="15.6640625" customWidth="1"/>
+    <col min="25" max="26" width="16.6640625" customWidth="1"/>
     <col min="27" max="27" width="13.83203125" style="30" customWidth="1"/>
-    <col min="28" max="28" width="34.33203125" style="51" customWidth="1"/>
-    <col min="29" max="29" width="33.6640625" style="51" customWidth="1"/>
-    <col min="30" max="30" width="4.6640625" style="51" customWidth="1"/>
-    <col min="31" max="31" width="12" style="51" customWidth="1"/>
-    <col min="32" max="32" width="14.6640625" style="51" customWidth="1"/>
-    <col min="33" max="33" width="6.6640625" style="51" customWidth="1"/>
-    <col min="34" max="34" width="8.1640625" style="51" customWidth="1"/>
-    <col min="35" max="35" width="20" style="51" customWidth="1"/>
-    <col min="36" max="36" width="7.1640625" style="51" customWidth="1"/>
-    <col min="37" max="37" width="7.6640625" style="51" customWidth="1"/>
-    <col min="38" max="38" width="6.6640625" style="51" customWidth="1"/>
-    <col min="39" max="39" width="5.6640625" style="51" customWidth="1"/>
-    <col min="40" max="40" width="11" style="51" customWidth="1"/>
-    <col min="41" max="41" width="6.6640625" style="51" customWidth="1"/>
-    <col min="42" max="42" width="9.6640625" style="51" customWidth="1"/>
-    <col min="43" max="43" width="8" style="51" customWidth="1"/>
-    <col min="44" max="44" width="8.1640625" style="51" customWidth="1"/>
-    <col min="45" max="45" width="19.1640625" style="51" customWidth="1"/>
-    <col min="46" max="46" width="15.6640625" style="51" customWidth="1"/>
-    <col min="47" max="1025" width="8.6640625" style="51" customWidth="1"/>
+    <col min="28" max="28" width="34.33203125" customWidth="1"/>
+    <col min="29" max="29" width="33.6640625" customWidth="1"/>
+    <col min="30" max="30" width="4.6640625" customWidth="1"/>
+    <col min="31" max="31" width="12" customWidth="1"/>
+    <col min="32" max="32" width="14.6640625" customWidth="1"/>
+    <col min="33" max="33" width="6.6640625" customWidth="1"/>
+    <col min="34" max="34" width="8.1640625" customWidth="1"/>
+    <col min="35" max="35" width="20" customWidth="1"/>
+    <col min="36" max="36" width="7.1640625" customWidth="1"/>
+    <col min="37" max="37" width="7.6640625" customWidth="1"/>
+    <col min="38" max="38" width="6.6640625" customWidth="1"/>
+    <col min="39" max="39" width="5.6640625" customWidth="1"/>
+    <col min="40" max="40" width="11" customWidth="1"/>
+    <col min="41" max="41" width="6.6640625" customWidth="1"/>
+    <col min="42" max="42" width="9.6640625" customWidth="1"/>
+    <col min="43" max="43" width="8" customWidth="1"/>
+    <col min="44" max="44" width="8.1640625" customWidth="1"/>
+    <col min="45" max="45" width="19.1640625" customWidth="1"/>
+    <col min="46" max="46" width="15.6640625" customWidth="1"/>
+    <col min="47" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A1" s="49"/>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="77" t="s">
         <v>250</v>
       </c>
-      <c r="C1" s="77"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="83"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="81"/>
       <c r="F1" s="36" t="s">
         <v>251</v>
       </c>
-      <c r="G1" s="52"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54"/>
-      <c r="AA1" s="56"/>
-      <c r="AB1" s="54"/>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="54"/>
-      <c r="AF1" s="54"/>
-      <c r="AG1" s="54"/>
-      <c r="AH1" s="54"/>
-      <c r="AI1" s="54"/>
-      <c r="AJ1" s="54"/>
-      <c r="AK1" s="54"/>
-      <c r="AL1" s="54"/>
-      <c r="AM1" s="54"/>
-      <c r="AN1" s="54"/>
-      <c r="AO1" s="54"/>
-      <c r="AP1" s="54"/>
-      <c r="AQ1" s="54"/>
-      <c r="AR1" s="54"/>
-      <c r="AS1" s="54"/>
-      <c r="AT1" s="55"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="52"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="53"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+      <c r="T1" s="53"/>
+      <c r="U1" s="53"/>
+      <c r="V1" s="53"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="53"/>
+      <c r="Y1" s="53"/>
+      <c r="Z1" s="53"/>
+      <c r="AA1" s="55"/>
+      <c r="AB1" s="53"/>
+      <c r="AC1" s="53"/>
+      <c r="AD1" s="53"/>
+      <c r="AE1" s="53"/>
+      <c r="AF1" s="53"/>
+      <c r="AG1" s="53"/>
+      <c r="AH1" s="53"/>
+      <c r="AI1" s="53"/>
+      <c r="AJ1" s="53"/>
+      <c r="AK1" s="53"/>
+      <c r="AL1" s="53"/>
+      <c r="AM1" s="53"/>
+      <c r="AN1" s="53"/>
+      <c r="AO1" s="53"/>
+      <c r="AP1" s="53"/>
+      <c r="AQ1" s="53"/>
+      <c r="AR1" s="53"/>
+      <c r="AS1" s="53"/>
+      <c r="AT1" s="54"/>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A2" s="50"/>
-      <c r="B2" s="80"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="76" t="s">
+      <c r="B2" s="78"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="74" t="s">
         <v>161</v>
       </c>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="84" t="s">
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="82" t="s">
         <v>173</v>
       </c>
-      <c r="M2" s="77"/>
-      <c r="N2" s="78"/>
-      <c r="O2" s="84" t="s">
+      <c r="M2" s="75"/>
+      <c r="N2" s="76"/>
+      <c r="O2" s="82" t="s">
         <v>180</v>
       </c>
-      <c r="P2" s="77"/>
-      <c r="Q2" s="78"/>
-      <c r="R2" s="76" t="s">
+      <c r="P2" s="75"/>
+      <c r="Q2" s="76"/>
+      <c r="R2" s="74" t="s">
         <v>185</v>
       </c>
-      <c r="S2" s="77"/>
-      <c r="T2" s="77"/>
-      <c r="U2" s="77"/>
-      <c r="V2" s="78"/>
-      <c r="W2" s="76" t="s">
+      <c r="S2" s="75"/>
+      <c r="T2" s="75"/>
+      <c r="U2" s="75"/>
+      <c r="V2" s="76"/>
+      <c r="W2" s="74" t="s">
         <v>196</v>
       </c>
-      <c r="X2" s="77"/>
-      <c r="Y2" s="78"/>
-      <c r="Z2" s="76" t="s">
+      <c r="X2" s="75"/>
+      <c r="Y2" s="76"/>
+      <c r="Z2" s="74" t="s">
         <v>203</v>
       </c>
-      <c r="AA2" s="77"/>
-      <c r="AB2" s="77"/>
-      <c r="AC2" s="77"/>
-      <c r="AD2" s="77"/>
-      <c r="AE2" s="77"/>
-      <c r="AF2" s="77"/>
-      <c r="AG2" s="77"/>
-      <c r="AH2" s="77"/>
-      <c r="AI2" s="78"/>
-      <c r="AJ2" s="76" t="s">
+      <c r="AA2" s="75"/>
+      <c r="AB2" s="75"/>
+      <c r="AC2" s="75"/>
+      <c r="AD2" s="75"/>
+      <c r="AE2" s="75"/>
+      <c r="AF2" s="75"/>
+      <c r="AG2" s="75"/>
+      <c r="AH2" s="75"/>
+      <c r="AI2" s="76"/>
+      <c r="AJ2" s="74" t="s">
         <v>224</v>
       </c>
-      <c r="AK2" s="77"/>
-      <c r="AL2" s="77"/>
-      <c r="AM2" s="77"/>
-      <c r="AN2" s="77"/>
-      <c r="AO2" s="77"/>
-      <c r="AP2" s="77"/>
-      <c r="AQ2" s="77"/>
-      <c r="AR2" s="77"/>
-      <c r="AS2" s="78"/>
+      <c r="AK2" s="75"/>
+      <c r="AL2" s="75"/>
+      <c r="AM2" s="75"/>
+      <c r="AN2" s="75"/>
+      <c r="AO2" s="75"/>
+      <c r="AP2" s="75"/>
+      <c r="AQ2" s="75"/>
+      <c r="AR2" s="75"/>
+      <c r="AS2" s="76"/>
     </row>
     <row r="3" spans="1:46" ht="26" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="37" t="s">
@@ -6928,7 +6929,7 @@
       <c r="Z3" s="47" t="s">
         <v>204</v>
       </c>
-      <c r="AA3" s="57" t="s">
+      <c r="AA3" s="56" t="s">
         <v>206</v>
       </c>
       <c r="AB3" s="44" t="s">
@@ -7056,7 +7057,7 @@
       <c r="M7" t="s">
         <v>256</v>
       </c>
-      <c r="Z7" s="58"/>
+      <c r="Z7" s="57"/>
     </row>
     <row r="8" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -7841,7 +7842,7 @@
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A54" s="51" t="s">
+      <c r="A54" t="s">
         <v>761</v>
       </c>
       <c r="F54" t="s">
@@ -7858,7 +7859,7 @@
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A55" s="51" t="s">
+      <c r="A55" t="s">
         <v>761</v>
       </c>
       <c r="F55" t="s">
@@ -7875,7 +7876,7 @@
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A56" s="51" t="s">
+      <c r="A56" t="s">
         <v>761</v>
       </c>
       <c r="F56" t="s">
@@ -7892,7 +7893,7 @@
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A57" s="51" t="s">
+      <c r="A57" t="s">
         <v>761</v>
       </c>
       <c r="F57" t="s">
@@ -7909,7 +7910,7 @@
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A58" s="51" t="s">
+      <c r="A58" t="s">
         <v>761</v>
       </c>
       <c r="F58" t="s">
@@ -7926,7 +7927,7 @@
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A59" s="51" t="s">
+      <c r="A59" t="s">
         <v>761</v>
       </c>
       <c r="F59" t="s">
@@ -7943,7 +7944,7 @@
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A60" s="51" t="s">
+      <c r="A60" t="s">
         <v>761</v>
       </c>
       <c r="F60" t="s">
@@ -7960,7 +7961,7 @@
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A61" s="51" t="s">
+      <c r="A61" t="s">
         <v>761</v>
       </c>
       <c r="F61" t="s">
@@ -7977,7 +7978,7 @@
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A62" s="51" t="s">
+      <c r="A62" t="s">
         <v>761</v>
       </c>
       <c r="F62" t="s">
@@ -7994,7 +7995,7 @@
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A63" s="51" t="s">
+      <c r="A63" t="s">
         <v>761</v>
       </c>
       <c r="F63" t="s">
@@ -8011,7 +8012,7 @@
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A64" s="51" t="s">
+      <c r="A64" t="s">
         <v>761</v>
       </c>
       <c r="F64" t="s">
@@ -8028,7 +8029,7 @@
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A65" s="51" t="s">
+      <c r="A65" t="s">
         <v>761</v>
       </c>
       <c r="F65" t="s">
@@ -8045,7 +8046,7 @@
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A66" s="51" t="s">
+      <c r="A66" t="s">
         <v>761</v>
       </c>
       <c r="F66" t="s">
@@ -8062,7 +8063,7 @@
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A67" s="51" t="s">
+      <c r="A67" t="s">
         <v>761</v>
       </c>
       <c r="F67" t="s">
@@ -8079,7 +8080,7 @@
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A68" s="51" t="s">
+      <c r="A68" t="s">
         <v>761</v>
       </c>
       <c r="F68" t="s">
@@ -8096,7 +8097,7 @@
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A69" s="51" t="s">
+      <c r="A69" t="s">
         <v>761</v>
       </c>
       <c r="F69" t="s">
@@ -8113,7 +8114,7 @@
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A70" s="51" t="s">
+      <c r="A70" t="s">
         <v>761</v>
       </c>
       <c r="F70" t="s">
@@ -8130,7 +8131,7 @@
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A71" s="51" t="s">
+      <c r="A71" t="s">
         <v>761</v>
       </c>
       <c r="F71" t="s">
@@ -8147,7 +8148,7 @@
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A72" s="51" t="s">
+      <c r="A72" t="s">
         <v>761</v>
       </c>
       <c r="F72" t="s">
@@ -8164,7 +8165,7 @@
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A73" s="51" t="s">
+      <c r="A73" t="s">
         <v>761</v>
       </c>
       <c r="F73" t="s">
@@ -8181,7 +8182,7 @@
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A74" s="51" t="s">
+      <c r="A74" t="s">
         <v>761</v>
       </c>
       <c r="F74" t="s">
@@ -8198,7 +8199,7 @@
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A75" s="51" t="s">
+      <c r="A75" t="s">
         <v>761</v>
       </c>
       <c r="F75" t="s">
@@ -8215,7 +8216,7 @@
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A76" s="51" t="s">
+      <c r="A76" t="s">
         <v>761</v>
       </c>
       <c r="F76" t="s">
@@ -8232,7 +8233,7 @@
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A77" s="51" t="s">
+      <c r="A77" t="s">
         <v>761</v>
       </c>
       <c r="F77" t="s">
@@ -8249,7 +8250,7 @@
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A78" s="51" t="s">
+      <c r="A78" t="s">
         <v>761</v>
       </c>
       <c r="F78" t="s">
@@ -8266,7 +8267,7 @@
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A79" s="51" t="s">
+      <c r="A79" t="s">
         <v>761</v>
       </c>
       <c r="F79" t="s">
@@ -8283,7 +8284,7 @@
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A80" s="51" t="s">
+      <c r="A80" t="s">
         <v>761</v>
       </c>
       <c r="F80" t="s">
@@ -8300,7 +8301,7 @@
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A81" s="51" t="s">
+      <c r="A81" t="s">
         <v>761</v>
       </c>
       <c r="F81" t="s">
@@ -8317,7 +8318,7 @@
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A82" s="51" t="s">
+      <c r="A82" t="s">
         <v>761</v>
       </c>
       <c r="F82" t="s">
@@ -8334,7 +8335,7 @@
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A83" s="51" t="s">
+      <c r="A83" t="s">
         <v>761</v>
       </c>
       <c r="F83" t="s">
@@ -8351,7 +8352,7 @@
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A84" s="51" t="s">
+      <c r="A84" t="s">
         <v>761</v>
       </c>
       <c r="F84" t="s">
@@ -8368,7 +8369,7 @@
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A85" s="51" t="s">
+      <c r="A85" t="s">
         <v>761</v>
       </c>
       <c r="F85" t="s">
@@ -8385,7 +8386,7 @@
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A86" s="51" t="s">
+      <c r="A86" t="s">
         <v>761</v>
       </c>
       <c r="F86" t="s">
@@ -8402,7 +8403,7 @@
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A87" s="51" t="s">
+      <c r="A87" t="s">
         <v>761</v>
       </c>
       <c r="F87" t="s">
@@ -8419,7 +8420,7 @@
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A88" s="51" t="s">
+      <c r="A88" t="s">
         <v>761</v>
       </c>
       <c r="F88" t="s">
@@ -8436,7 +8437,7 @@
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A89" s="51" t="s">
+      <c r="A89" t="s">
         <v>761</v>
       </c>
       <c r="F89" t="s">
@@ -8453,7 +8454,7 @@
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A90" s="51" t="s">
+      <c r="A90" t="s">
         <v>761</v>
       </c>
       <c r="F90" t="s">
@@ -8470,7 +8471,7 @@
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A91" s="51" t="s">
+      <c r="A91" t="s">
         <v>761</v>
       </c>
       <c r="F91" t="s">
@@ -8487,7 +8488,7 @@
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A92" s="51" t="s">
+      <c r="A92" t="s">
         <v>761</v>
       </c>
       <c r="F92" t="s">
@@ -8504,7 +8505,7 @@
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A93" s="51" t="s">
+      <c r="A93" t="s">
         <v>761</v>
       </c>
       <c r="F93" t="s">
@@ -8521,7 +8522,7 @@
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A94" s="51" t="s">
+      <c r="A94" t="s">
         <v>761</v>
       </c>
       <c r="F94" t="s">
@@ -8538,7 +8539,7 @@
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A95" s="51" t="s">
+      <c r="A95" t="s">
         <v>761</v>
       </c>
       <c r="F95" t="s">
@@ -8555,7 +8556,7 @@
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A96" s="51" t="s">
+      <c r="A96" t="s">
         <v>761</v>
       </c>
       <c r="F96" t="s">
@@ -8572,7 +8573,7 @@
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A97" s="51" t="s">
+      <c r="A97" t="s">
         <v>761</v>
       </c>
       <c r="F97" t="s">
@@ -8589,7 +8590,7 @@
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A98" s="51" t="s">
+      <c r="A98" t="s">
         <v>761</v>
       </c>
       <c r="F98" t="s">
@@ -8606,7 +8607,7 @@
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A99" s="51" t="s">
+      <c r="A99" t="s">
         <v>761</v>
       </c>
       <c r="F99" t="s">
@@ -8623,7 +8624,7 @@
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A100" s="51" t="s">
+      <c r="A100" t="s">
         <v>761</v>
       </c>
       <c r="F100" t="s">
@@ -8640,7 +8641,7 @@
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A101" s="51" t="s">
+      <c r="A101" t="s">
         <v>761</v>
       </c>
       <c r="F101" t="s">
@@ -8657,7 +8658,7 @@
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A102" s="51" t="s">
+      <c r="A102" t="s">
         <v>761</v>
       </c>
       <c r="F102" t="s">
@@ -8674,7 +8675,7 @@
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A103" s="51" t="s">
+      <c r="A103" t="s">
         <v>761</v>
       </c>
       <c r="F103" t="s">
@@ -8717,15 +8718,15 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:AMK5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" style="51" customWidth="1"/>
-    <col min="2" max="2" width="114.6640625" style="51" customWidth="1"/>
-    <col min="3" max="1025" width="8.6640625" style="51" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="114.6640625" customWidth="1"/>
+    <col min="3" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>